<commit_message>
changes to make predictions for categories
</commit_message>
<xml_diff>
--- a/all_accuracy.xlsx
+++ b/all_accuracy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Racec\PycharmProjects\network-trace-application-predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FZTHWP\PycharmProjects\network-trace-application-predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6921F0-598A-4BC0-8667-741946A70ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED261356-9C0D-43D4-8B8E-ABDBA93A5278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1830" windowWidth="26205" windowHeight="11385" xr2:uid="{99BEECD5-61B8-4C28-9FA7-93FB32CE2292}"/>
+    <workbookView xWindow="30" yWindow="2340" windowWidth="21600" windowHeight="11370" xr2:uid="{99BEECD5-61B8-4C28-9FA7-93FB32CE2292}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Packet Name</t>
   </si>
@@ -48,9 +47,6 @@
     <t>Keras</t>
   </si>
   <si>
-    <t>Linear Regression</t>
-  </si>
-  <si>
     <t>XGBoost</t>
   </si>
   <si>
@@ -64,9 +60,6 @@
   </si>
   <si>
     <t>LTE_PDCP_DL_Stats</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>*NOTE: Linear Regression only calculated by R2 Score</t>
@@ -446,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E73857B-5E1E-4511-9243-F8FCA3951084}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,11 +450,10 @@
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,16 +469,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>0.33600000000000002</v>
@@ -498,18 +487,15 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="E2">
-        <v>0.06</v>
-      </c>
-      <c r="F2">
         <v>0.23499999999999999</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>13</v>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.16500000000000001</v>
@@ -521,18 +507,15 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="E3">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="F3">
         <v>0.1762</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>14</v>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.435</v>
@@ -543,16 +526,13 @@
       <c r="D4">
         <v>0.502</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
+      <c r="E4">
         <v>0.371</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.61199999999999999</v>
@@ -563,16 +543,13 @@
       <c r="D5" s="2">
         <v>0.76600000000000001</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
-      </c>
-      <c r="F5">
-        <v>0.59799999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6">
         <v>0.40600000000000003</v>
@@ -584,9 +561,6 @@
         <v>0.34799999999999998</v>
       </c>
       <c r="E6">
-        <v>-0.26800000000000002</v>
-      </c>
-      <c r="F6">
         <v>0.23200000000000001</v>
       </c>
     </row>

</xml_diff>